<commit_message>
Method to compare dates
</commit_message>
<xml_diff>
--- a/test/data/BigIssueRostering.xlsx
+++ b/test/data/BigIssueRostering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joao/Documents/GitHub/swen90014-2019-bi-bilby/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E8AE98-0DD5-3B44-84A0-2FE434AA6FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FAAA94-8610-2946-A041-7ADABBBBA8A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8258,10 +8258,10 @@
   <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomRight" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8627,7 +8627,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="10" t="s">
@@ -8638,7 +8638,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>156</v>
@@ -8646,35 +8646,31 @@
       <c r="I5" s="11">
         <v>0.375</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="38">
         <v>0.5</v>
       </c>
-      <c r="K5" s="11">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="L5" s="11">
-        <v>0.66666666666666663</v>
-      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11">
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="P5" s="11">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
+        <v>0.625</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
-      <c r="W5" s="35">
-        <v>43503</v>
-      </c>
-      <c r="X5" s="35">
-        <v>43506</v>
-      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
@@ -8697,7 +8693,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="10" t="s">
@@ -8708,7 +8704,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>156</v>
@@ -8716,31 +8712,35 @@
       <c r="I6" s="11">
         <v>0.375</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="11">
         <v>0.5</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="K6" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
-      <c r="O6" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="P6" s="40">
-        <v>0.625</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="R6" s="11">
-        <v>0.58333333333333337</v>
-      </c>
+      <c r="O6" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
+      <c r="W6" s="35">
+        <v>43503</v>
+      </c>
+      <c r="X6" s="35">
+        <v>43506</v>
+      </c>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
@@ -10638,8 +10638,12 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:V43 I4:J4 I3 I11:I12 O7:R7 Q27:R27 P25:P26 J29:J30 R28:R43 I31:J43 O19:P21 P22:P23 O24:P24 O27:P43 K18:L18 R25:R26 I13:J14 I5:I6 I7:J8 I9 I10:J10 I19:J28 I2:L2 I15 I16:J17 M2:N43 K14:L14 Q17:R24 J5 K20:L43 O9:P9 O3:P5 P16:R16 Q2:R6 Q8:R15 K3:L6 K11:L11" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3 I11:I12 O7:R7 Q27:R27 P25:P26 J29:J30 R28:R43 I31:J43 O19:P21 P22:P23 O24:P24 O27:P43 K18:L18 R25:R26 I13:J14 I9 I10:J10 I19:J28 I2:L2 I15 I16:J17 K14:L14 Q17:R24 K11:L11 K20:L43 O9:P9 O3:P6 P16:R16 Q2:R6 Q8:R15 K3:L6 I4:J8 M2:N43 S2:V43" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>0.375</formula1>
+      <formula2>0.708333333333333</formula2>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O25:O26 Q1 Q28:Q1048576 I29:I30 O22:O23 Q25:Q26 O16" xr:uid="{00000000-0002-0000-0400-000004000000}">
+      <formula1>0.354166666666667</formula1>
       <formula2>0.708333333333333</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F43" xr:uid="{00000000-0002-0000-0400-000001000000}">
@@ -10651,15 +10655,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A43" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>"Facilitator,Guest Speaker"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O25:O26 Q1 Q28:Q1048576 I29:I30 O22:O23 Q25:Q26 O16" xr:uid="{00000000-0002-0000-0400-000004000000}">
-      <formula1>0.354166666666667</formula1>
-      <formula2>0.708333333333333</formula2>
-    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="D3:D15" r:id="rId2" display="www.www@sss.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="D16:D19" r:id="rId3" display="www.www@sss.com" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="D16:D19" r:id="rId2" display="www.www@sss.com" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>